<commit_message>
Improving OCR pipeline + adding words to main dict
</commit_message>
<xml_diff>
--- a/data/tables/main.xlsx
+++ b/data/tables/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\Tsakonian tools\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69EFF31-5C28-4455-8DB5-5E831462D087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C2100C-2D20-41FD-91FF-356200672972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14490" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7305" yWindow="900" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="935">
   <si>
     <t>tsakonian</t>
   </si>
@@ -2522,13 +2522,316 @@
   </si>
   <si>
     <t>κρεβάτι</t>
+  </si>
+  <si>
+    <t>κοϊθίνι</t>
+  </si>
+  <si>
+    <t>κοφίνι</t>
+  </si>
+  <si>
+    <t>ντρυνικό</t>
+  </si>
+  <si>
+    <t>μεγάλο καλάθι, τρυγοκόφινο</t>
+  </si>
+  <si>
+    <t>σάκ̇ο</t>
+  </si>
+  <si>
+    <t>σακί</t>
+  </si>
+  <si>
+    <t>μάτουκα</t>
+  </si>
+  <si>
+    <t>τσάπα</t>
+  </si>
+  <si>
+    <t>ξινιάρι</t>
+  </si>
+  <si>
+    <t>µπίκο</t>
+  </si>
+  <si>
+    <t>κασµάς</t>
+  </si>
+  <si>
+    <t>έρατσ̌ε</t>
+  </si>
+  <si>
+    <t>αλέτρι</t>
+  </si>
+  <si>
+    <t>σ̌ίνακα</t>
+  </si>
+  <si>
+    <t>δικριάνι</t>
+  </si>
+  <si>
+    <t>φκιάρι</t>
+  </si>
+  <si>
+    <t>φτυάρι</t>
+  </si>
+  <si>
+    <t>κακίστρι</t>
+  </si>
+  <si>
+    <t>καπίστρι</t>
+  </si>
+  <si>
+    <t>τριχία</t>
+  </si>
+  <si>
+    <t>τριχιά</t>
+  </si>
+  <si>
+    <t>γκιτσία</t>
+  </si>
+  <si>
+    <t>πιστιά</t>
+  </si>
+  <si>
+    <t>δίγκα</t>
+  </si>
+  <si>
+    <t>ίγκλα</t>
+  </si>
+  <si>
+    <t>πράνα</t>
+  </si>
+  <si>
+    <t>κόπανος</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ατσίμπτανε</t>
+  </si>
+  <si>
+    <t>σφενδάμι</t>
+  </si>
+  <si>
+    <t>χαρουπία</t>
+  </si>
+  <si>
+    <t>χαρουπιά</t>
+  </si>
+  <si>
+    <t>αχλαδιά</t>
+  </si>
+  <si>
+    <t>συντζά</t>
+  </si>
+  <si>
+    <t>συκιά</t>
+  </si>
+  <si>
+    <t>μουρία</t>
+  </si>
+  <si>
+    <t>µουριά</t>
+  </si>
+  <si>
+    <t>λεµον̇ία</t>
+  </si>
+  <si>
+    <t>λεµονιά</t>
+  </si>
+  <si>
+    <t>πορτοκαλ̣ία</t>
+  </si>
+  <si>
+    <t>πορτοκαλιά</t>
+  </si>
+  <si>
+    <t>τσ̇υδωνία</t>
+  </si>
+  <si>
+    <t>κυδωνιά</t>
+  </si>
+  <si>
+    <t>καϊσία</t>
+  </si>
+  <si>
+    <t>καϊσιά (βερυκοκιά)</t>
+  </si>
+  <si>
+    <t>καζ̌ά</t>
+  </si>
+  <si>
+    <t>καρυδιά</t>
+  </si>
+  <si>
+    <t>κράµα</t>
+  </si>
+  <si>
+    <t>κλήµα</t>
+  </si>
+  <si>
+    <t>αλιοχρά</t>
+  </si>
+  <si>
+    <t>αγριαχλαδιά (γκορτσιά)</t>
+  </si>
+  <si>
+    <t>πρίνε</t>
+  </si>
+  <si>
+    <t>πουρνάρι</t>
+  </si>
+  <si>
+    <t>τσ̌ούα</t>
+  </si>
+  <si>
+    <t>βελανιδιά</t>
+  </si>
+  <si>
+    <t>μουνταλία</t>
+  </si>
+  <si>
+    <t>µυρτιά</t>
+  </si>
+  <si>
+    <t>φίλ̣υτσ̌ε</t>
+  </si>
+  <si>
+    <t>γλαντινιά</t>
+  </si>
+  <si>
+    <t>κούμαρε</t>
+  </si>
+  <si>
+    <t>κουµαριά</t>
+  </si>
+  <si>
+    <t>ακόρβατ̇ε</t>
+  </si>
+  <si>
+    <t>βάτο</t>
+  </si>
+  <si>
+    <t>φτερένισε</t>
+  </si>
+  <si>
+    <t>κοκορεβιθιά</t>
+  </si>
+  <si>
+    <t>π̇άντι</t>
+  </si>
+  <si>
+    <t>σπάρτο</t>
+  </si>
+  <si>
+    <t>απ̇αλία</t>
+  </si>
+  <si>
+    <t>σφαλάχτρι</t>
+  </si>
+  <si>
+    <t>κουκουτσία</t>
+  </si>
+  <si>
+    <t>κουτσουπιά</t>
+  </si>
+  <si>
+    <t>έατε</t>
+  </si>
+  <si>
+    <t>έλατο</t>
+  </si>
+  <si>
+    <t>τσίνε</t>
+  </si>
+  <si>
+    <t>σχίντο</t>
+  </si>
+  <si>
+    <t>νυγδαλ̣ία</t>
+  </si>
+  <si>
+    <t>αμυγδαλιά</t>
+  </si>
+  <si>
+    <t>κρέµµου</t>
+  </si>
+  <si>
+    <t>κρεμμύδι</t>
+  </si>
+  <si>
+    <t>απ̇άρα</t>
+  </si>
+  <si>
+    <t>καρναμπίτσ̇ι</t>
+  </si>
+  <si>
+    <t>κουνουπίδι</t>
+  </si>
+  <si>
+    <t>ντουµάτα</t>
+  </si>
+  <si>
+    <t>δέηµα</t>
+  </si>
+  <si>
+    <t>κοντό κολοκύθι</t>
+  </si>
+  <si>
+    <t>μακουνία</t>
+  </si>
+  <si>
+    <t>παπαρούνα</t>
+  </si>
+  <si>
+    <t>κοκαλία</t>
+  </si>
+  <si>
+    <t>καυκαλήθρα</t>
+  </si>
+  <si>
+    <t>κ̇άντζικα</t>
+  </si>
+  <si>
+    <t>μυρώνι</t>
+  </si>
+  <si>
+    <t>ζ̌ογκό</t>
+  </si>
+  <si>
+    <t>τζοχός</t>
+  </si>
+  <si>
+    <t>κόκ̇ο</t>
+  </si>
+  <si>
+    <t>ατζίναρε</t>
+  </si>
+  <si>
+    <t>ελία</t>
+  </si>
+  <si>
+    <t>άρτουµα</t>
+  </si>
+  <si>
+    <t>π̇ίτια</t>
+  </si>
+  <si>
+    <t>χυλοπίτες</t>
+  </si>
+  <si>
+    <t>φαέ</t>
+  </si>
+  <si>
+    <t>στάρι</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2553,6 +2856,12 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2647,6 +2956,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -2662,13 +2978,6 @@
         <sz val="14"/>
         <name val="Calibri"/>
       </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2712,8 +3021,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}" name="Tabla1" displayName="Tabla1" ref="A1:D421" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
-  <autoFilter ref="A1:D421" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}" name="Tabla1" displayName="Tabla1" ref="A1:D496" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="A1:D496" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D351">
     <sortCondition ref="A1:A351"/>
   </sortState>
@@ -3012,10 +3321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D421"/>
+  <dimension ref="A1:P496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A399" workbookViewId="0">
-      <selection activeCell="A422" sqref="A422"/>
+    <sheetView tabSelected="1" topLeftCell="A482" workbookViewId="0">
+      <selection activeCell="A491" sqref="A491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8560,7 +8869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A401" s="3" t="s">
         <v>798</v>
       </c>
@@ -8574,7 +8883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A402" s="3" t="s">
         <v>800</v>
       </c>
@@ -8588,7 +8897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A403" s="3" t="s">
         <v>802</v>
       </c>
@@ -8602,7 +8911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A404" s="2" t="s">
         <v>804</v>
       </c>
@@ -8616,7 +8925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A405" s="3" t="s">
         <v>806</v>
       </c>
@@ -8630,7 +8939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="406" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A406" s="3" t="s">
         <v>807</v>
       </c>
@@ -8642,7 +8951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="407" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A407" s="2" t="s">
         <v>809</v>
       </c>
@@ -8656,7 +8965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="408" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A408" s="3" t="s">
         <v>810</v>
       </c>
@@ -8670,7 +8979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="409" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A409" s="3" t="s">
         <v>812</v>
       </c>
@@ -8684,7 +8993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="410" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A410" s="3" t="s">
         <v>813</v>
       </c>
@@ -8698,7 +9007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="411" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A411" s="3" t="s">
         <v>814</v>
       </c>
@@ -8712,7 +9021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="412" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A412" s="3" t="s">
         <v>816</v>
       </c>
@@ -8726,7 +9035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="413" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A413" s="3" t="s">
         <v>46</v>
       </c>
@@ -8740,7 +9049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="414" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A414" s="3" t="s">
         <v>818</v>
       </c>
@@ -8753,8 +9062,11 @@
       <c r="D414" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="415" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="P414" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="415" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A415" s="3" t="s">
         <v>820</v>
       </c>
@@ -8764,9 +9076,11 @@
       <c r="C415" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="D415" s="3"/>
-    </row>
-    <row r="416" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D415" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A416" s="3" t="s">
         <v>822</v>
       </c>
@@ -8776,7 +9090,9 @@
       <c r="C416" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D416" s="3"/>
+      <c r="D416" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="417" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A417" s="3" t="s">
@@ -8788,7 +9104,9 @@
       <c r="C417" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="D417" s="3"/>
+      <c r="D417" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="418" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A418" s="3" t="s">
@@ -8800,7 +9118,9 @@
       <c r="C418" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D418" s="3"/>
+      <c r="D418" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="419" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A419" s="3" t="s">
@@ -8812,7 +9132,9 @@
       <c r="C419" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D419" s="3"/>
+      <c r="D419" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="420" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A420" s="3" t="s">
@@ -8824,7 +9146,9 @@
       <c r="C420" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D420" s="3"/>
+      <c r="D420" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="421" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A421" s="3" t="s">
@@ -8836,9 +9160,1060 @@
       <c r="C421" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D421" s="3"/>
+      <c r="D421" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A422" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="B422" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="C422" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="D422" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A423" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="B423" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="C423" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D423" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A424" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="B424" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="C424" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D424" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A425" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="B425" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="C425" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D425" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A426" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="B426" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="C426" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D426" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A427" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="B427" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="C427" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D427" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A428" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B428" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="C428" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D428" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A429" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="B429" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="C429" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D429" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A430" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="B430" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="C430" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="D430" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A431" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="B431" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="C431" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="D431" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A432" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="B432" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="C432" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D432" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A433" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="B433" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="C433" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D433" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A434" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="B434" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="C434" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D434" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A435" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="B435" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="C435" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D435" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A436" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="B436" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="C436" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D436" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A437" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B437" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C437" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D437" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A438" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="B438" s="3" t="s">
+        <v>865</v>
+      </c>
+      <c r="C438" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D438" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A439" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B439" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="C439" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D439" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A440" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="B440" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="C440" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D440" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A441" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="B441" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="C441" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D441" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A442" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="B442" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="C442" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D442" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A443" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="B443" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="C443" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D443" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A444" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="B444" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="C444" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D444" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A445" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="B445" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="C445" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D445" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A446" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="B446" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="C446" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D446" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A447" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="B447" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="C447" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D447" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A448" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B448" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C448" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D448" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A449" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="B449" s="3" t="s">
+        <v>865</v>
+      </c>
+      <c r="C449" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D449" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A450" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B450" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="C450" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D450" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A451" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="B451" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="C451" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D451" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A452" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="B452" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="C452" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D452" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A453" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="B453" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="C453" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D453" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A454" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="B454" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="C454" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D454" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A455" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="B455" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="C455" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D455" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A456" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="B456" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="C456" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D456" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A457" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="B457" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="C457" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D457" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A458" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="B458" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="C458" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D458" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A459" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="B459" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="C459" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D459" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A460" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="B460" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="C460" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D460" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A461" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="B461" s="3" t="s">
+        <v>888</v>
+      </c>
+      <c r="C461" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D461" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A462" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="B462" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="C462" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D462" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A463" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="B463" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="C463" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D463" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A464" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="B464" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="C464" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D464" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A465" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="B465" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="C465" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D465" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A466" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="B466" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="C466" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D466" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A467" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="B467" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="C467" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D467" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A468" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="B468" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="C468" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D468" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A469" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="B469" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="C469" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D469" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A470" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B470" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="C470" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D470" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A471" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="B471" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="C471" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D471" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A472" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="B472" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="C472" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D472" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A473" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="B473" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="C473" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D473" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A474" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B474" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C474" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D474" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A475" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="B475" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C475" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D475" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A476" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="B476" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="C476" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D476" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A477" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="B477" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="C477" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D477" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A478" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B478" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C478" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D478" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A479" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B479" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="C479" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D479" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A480" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="B480" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="C480" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D480" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A481" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="B481" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="C481" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D481" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A482" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="B482" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="C482" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D482" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A483" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B483" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C483" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D483" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A484" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="B484" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="C484" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D484" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A485" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="B485" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C485" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D485" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A486" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="B486" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C486" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D486" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A487" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="B487" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C487" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D487" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A488" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="B488" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="C488" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D488" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A489" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B489" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C489" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D489" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A490" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B490" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C490" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D490" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A491" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B491" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C491" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D491" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A492" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="B492" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C492" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D492" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A493" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B493" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C493" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D493" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A494" s="3" t="s">
+        <v>931</v>
+      </c>
+      <c r="B494" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="C494" s="3"/>
+      <c r="D494" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A495" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="B495" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="C495" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D495" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A496" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="B496" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="C496" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D496" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Adding reading words from Google Lens
</commit_message>
<xml_diff>
--- a/data/tables/main.xlsx
+++ b/data/tables/main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\Tsakonian tools\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C2100C-2D20-41FD-91FF-356200672972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCCEC4B-23B8-4CE8-88F6-69644EE82B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="900" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="953">
   <si>
     <t>tsakonian</t>
   </si>
@@ -2825,6 +2825,60 @@
   </si>
   <si>
     <t>στάρι</t>
+  </si>
+  <si>
+    <t>κουλίντζου</t>
+  </si>
+  <si>
+    <t>είδος ζυμαρικού</t>
+  </si>
+  <si>
+    <t>κολιούρα</t>
+  </si>
+  <si>
+    <t>πίτα που ψήνεται στην πλάνη</t>
+  </si>
+  <si>
+    <t>γριτσ̇έα</t>
+  </si>
+  <si>
+    <t>κουλούρα</t>
+  </si>
+  <si>
+    <t>κάζ̌υ</t>
+  </si>
+  <si>
+    <t>καρύδι</t>
+  </si>
+  <si>
+    <t>κουνάρι</t>
+  </si>
+  <si>
+    <t>σκυλάκι</t>
+  </si>
+  <si>
+    <t>μονάρι</t>
+  </si>
+  <si>
+    <t>μουλάρι</t>
+  </si>
+  <si>
+    <t>βου</t>
+  </si>
+  <si>
+    <t>βόδι</t>
+  </si>
+  <si>
+    <t>ρουφάλι</t>
+  </si>
+  <si>
+    <t>κατσικάκι</t>
+  </si>
+  <si>
+    <t>τσ̌άο</t>
+  </si>
+  <si>
+    <t>τραγί</t>
   </si>
 </sst>
 </file>
@@ -2856,6 +2910,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2956,13 +3011,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -2978,6 +3026,13 @@
         <sz val="14"/>
         <name val="Calibri"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3021,8 +3076,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}" name="Tabla1" displayName="Tabla1" ref="A1:D496" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
-  <autoFilter ref="A1:D496" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}" name="Tabla1" displayName="Tabla1" ref="A1:D524" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="A1:D524" xr:uid="{5EF29A5B-8D20-4CD7-8E92-F1C4AD49B7BE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D351">
     <sortCondition ref="A1:A351"/>
   </sortState>
@@ -3321,10 +3376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P496"/>
+  <dimension ref="A1:P524"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A482" workbookViewId="0">
-      <selection activeCell="A491" sqref="A491"/>
+    <sheetView tabSelected="1" topLeftCell="A508" workbookViewId="0">
+      <selection activeCell="A524" sqref="A524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10212,6 +10267,388 @@
         <v>1</v>
       </c>
     </row>
+    <row r="497" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A497" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B497" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C497" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D497" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A498" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B498" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C498" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D498" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A499" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B499" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C499" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D499" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A500" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B500" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C500" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D500" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A501" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="B501" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="C501" s="2"/>
+      <c r="D501" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A502" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B502" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="C502" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D502" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A503" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B503" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="C503" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D503" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A504" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B504" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C504" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D504" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A505" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="B505" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="C505" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D505" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A506" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C506" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D506" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A507" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B507" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C507" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D507" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A508" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="B508" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="C508" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="D508" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A509" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B509" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C509" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D509" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A510" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B510" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C510" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D510" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A511" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C511" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D511" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A512" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B512" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C512" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D512" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A513" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="B513" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="C513" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="D513" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A514" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B514" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C514" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="D514" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A515" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="B515" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="C515" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D515" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A516" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B516" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C516" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D516" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A517" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B517" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C517" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D517" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A518" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B518" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C518" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D518" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A519" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B519" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C519" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D519" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A520" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B520" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C520" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D520" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A521" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B521" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C521" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D521" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A522" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B522" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="C522" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="D522" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A523" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="B523" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="C523" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D523" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A524" s="2"/>
+      <c r="B524" s="2"/>
+      <c r="C524" s="2"/>
+      <c r="D524" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Adding support for keyboard extension
</commit_message>
<xml_diff>
--- a/data/tables/main.xlsx
+++ b/data/tables/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\TsakonianDB\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8DC75D-286B-44B8-8274-B95AC4C2E32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C885B99-D7DC-4A07-B9DD-D1537A5357E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="6900" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2313" uniqueCount="1508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="1520">
   <si>
     <t>tsakonian</t>
   </si>
@@ -4544,6 +4544,42 @@
   </si>
   <si>
     <t>πλεύρα</t>
+  </si>
+  <si>
+    <t>κείνα</t>
+  </si>
+  <si>
+    <t>στσεγκουμένε</t>
+  </si>
+  <si>
+    <t>σκέφτομαι</t>
+  </si>
+  <si>
+    <t>ιδέα</t>
+  </si>
+  <si>
+    <t>πιο</t>
+  </si>
+  <si>
+    <t>τσαπρούκ̇ου</t>
+  </si>
+  <si>
+    <t>ξαπλώνω</t>
+  </si>
+  <si>
+    <t>φόλα</t>
+  </si>
+  <si>
+    <t>ψοφού</t>
+  </si>
+  <si>
+    <t>ψοφώ</t>
+  </si>
+  <si>
+    <t>προχωρού</t>
+  </si>
+  <si>
+    <t>προχωράω</t>
   </si>
 </sst>
 </file>
@@ -4906,10 +4942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D804"/>
+  <dimension ref="A1:D812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A780" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A805" sqref="A805"/>
+    <sheetView tabSelected="1" topLeftCell="A796" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A813" sqref="A813"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15846,6 +15882,94 @@
         <v>37</v>
       </c>
     </row>
+    <row r="805" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A805" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B805" t="s">
+        <v>605</v>
+      </c>
+      <c r="C805" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="806" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A806" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B806" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C806" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="807" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A807" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B807" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C807" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="808" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A808" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B808" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C808" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="809" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A809" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B809" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C809" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A810" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B810" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C810" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A811" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B811" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C811" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="812" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A812" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B812" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C812" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>